<commit_message>
Relatório da atividade log
</commit_message>
<xml_diff>
--- a/Exercicios/U5C1Tarefas/datalog.xlsx
+++ b/Exercicios/U5C1Tarefas/datalog.xlsx
@@ -69,11 +69,8 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -688,6 +685,7 @@
         <c:dLbls>
           <c:showBubbleSize val="0"/>
           <c:showCatName val="0"/>
+          <c:showLeaderLines val="0"/>
           <c:showLegendKey val="0"/>
           <c:showPercent val="0"/>
           <c:showSerName val="0"/>
@@ -866,7 +864,7 @@
   </c:chart>
   <c:spPr bwMode="auto">
     <a:xfrm rot="0" flipH="0" flipV="0">
-      <a:off x="3625214" y="373379"/>
+      <a:off x="3695697" y="373378"/>
       <a:ext cx="8553449" cy="4577715"/>
     </a:xfrm>
     <a:prstGeom prst="rect">
@@ -1501,14 +1499,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main">
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>592453</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>601977</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>7619</xdr:rowOff>
+      <xdr:rowOff>7618</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>1904</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>11426</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>13333</xdr:rowOff>
     </xdr:to>
@@ -1520,7 +1518,7 @@
         </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm rot="0" flipH="0" flipV="0">
-        <a:off x="3625214" y="373379"/>
+        <a:off x="3695697" y="373378"/>
         <a:ext cx="8553449" cy="4577715"/>
       </xdr:xfrm>
       <a:graphic>
@@ -2022,21 +2020,23 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col customWidth="1" min="1" max="1" style="1" width="18.00390625"/>
+    <col customWidth="1" min="2" max="2" width="15.28125"/>
+    <col customWidth="1" min="3" max="3" width="13.00390625"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>45946.604247685187</v>
       </c>
       <c r="B2">
@@ -2047,7 +2047,7 @@
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>45946.604259259257</v>
       </c>
       <c r="B3">
@@ -2058,7 +2058,7 @@
       </c>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>45946.604270833333</v>
       </c>
       <c r="B4">
@@ -2069,7 +2069,7 @@
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>45946.60429398148</v>
       </c>
       <c r="B5">
@@ -2080,10 +2080,10 @@
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>45946.604305555556</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>24.620000000000001</v>
       </c>
       <c r="C6">
@@ -2091,10 +2091,10 @@
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>45946.604317129626</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>24.600000000000001</v>
       </c>
       <c r="C7">
@@ -2102,10 +2102,10 @@
       </c>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>45946.604328703703</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>24.609999999999999</v>
       </c>
       <c r="C8">
@@ -2113,10 +2113,10 @@
       </c>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>45946.604351851849</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>24.620000000000001</v>
       </c>
       <c r="C9">
@@ -2124,10 +2124,10 @@
       </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>45946.604363425926</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>24.629999999999999</v>
       </c>
       <c r="C10">
@@ -2135,10 +2135,10 @@
       </c>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>45946.604375000003</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>24.609999999999999</v>
       </c>
       <c r="C11">
@@ -2146,10 +2146,10 @@
       </c>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>45946.604386574072</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>24.609999999999999</v>
       </c>
       <c r="C12">
@@ -2157,10 +2157,10 @@
       </c>
     </row>
     <row r="13" ht="14.25">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>45946.604398148149</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>24.609999999999999</v>
       </c>
       <c r="C13">
@@ -2168,10 +2168,10 @@
       </c>
     </row>
     <row r="14" ht="14.25">
-      <c r="A14" s="3">
+      <c r="A14" s="2">
         <v>45946.604421296295</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <v>24.609999999999999</v>
       </c>
       <c r="C14">
@@ -2179,10 +2179,10 @@
       </c>
     </row>
     <row r="15" ht="14.25">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>45946.604432870372</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>24.629999999999999</v>
       </c>
       <c r="C15">
@@ -2190,10 +2190,10 @@
       </c>
     </row>
     <row r="16" ht="14.25">
-      <c r="A16" s="3">
+      <c r="A16" s="2">
         <v>45946.604444444441</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>24.640000000000001</v>
       </c>
       <c r="C16">
@@ -2201,10 +2201,10 @@
       </c>
     </row>
     <row r="17" ht="14.25">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>45946.604456018518</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <v>24.66</v>
       </c>
       <c r="C17">
@@ -2212,10 +2212,10 @@
       </c>
     </row>
     <row r="18" ht="14.25">
-      <c r="A18" s="3">
+      <c r="A18" s="2">
         <v>45946.604479166665</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <v>24.670000000000002</v>
       </c>
       <c r="C18">
@@ -2223,10 +2223,10 @@
       </c>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19" s="3">
+      <c r="A19" s="2">
         <v>45946.604490740741</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="3">
         <v>24.66</v>
       </c>
       <c r="C19">
@@ -2234,10 +2234,10 @@
       </c>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="3">
+      <c r="A20" s="2">
         <v>45946.604502314818</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="3">
         <v>24.68</v>
       </c>
       <c r="C20">
@@ -2245,10 +2245,10 @@
       </c>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" s="3">
+      <c r="A21" s="2">
         <v>45946.604513888888</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="3">
         <v>24.690000000000001</v>
       </c>
       <c r="C21">
@@ -2256,10 +2256,10 @@
       </c>
     </row>
     <row r="22" ht="14.25">
-      <c r="A22" s="3">
+      <c r="A22" s="2">
         <v>45946.604525462964</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="3">
         <v>24.690000000000001</v>
       </c>
       <c r="C22">
@@ -2267,10 +2267,10 @@
       </c>
     </row>
     <row r="23" ht="14.25">
-      <c r="A23" s="3">
+      <c r="A23" s="2">
         <v>45946.604548611111</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="3">
         <v>24.699999999999999</v>
       </c>
       <c r="C23">
@@ -2278,10 +2278,10 @@
       </c>
     </row>
     <row r="24" ht="14.25">
-      <c r="A24" s="3">
+      <c r="A24" s="2">
         <v>45946.604560185187</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="3">
         <v>24.699999999999999</v>
       </c>
       <c r="C24">
@@ -2289,10 +2289,10 @@
       </c>
     </row>
     <row r="25" ht="14.25">
-      <c r="A25" s="3">
+      <c r="A25" s="2">
         <v>45946.604571759257</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="3">
         <v>24.710000000000001</v>
       </c>
       <c r="C25">
@@ -2300,10 +2300,10 @@
       </c>
     </row>
     <row r="26" ht="14.25">
-      <c r="A26" s="3">
+      <c r="A26" s="2">
         <v>45946.604583333334</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="3">
         <v>24.73</v>
       </c>
       <c r="C26">
@@ -2311,10 +2311,10 @@
       </c>
     </row>
     <row r="27" ht="14.25">
-      <c r="A27" s="3">
+      <c r="A27" s="2">
         <v>45946.60460648148</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="3">
         <v>24.760000000000002</v>
       </c>
       <c r="C27">
@@ -2322,10 +2322,10 @@
       </c>
     </row>
     <row r="28" ht="14.25">
-      <c r="A28" s="3">
+      <c r="A28" s="2">
         <v>45946.604618055557</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="3">
         <v>25.43</v>
       </c>
       <c r="C28">
@@ -2333,10 +2333,10 @@
       </c>
     </row>
     <row r="29" ht="14.25">
-      <c r="A29" s="3">
+      <c r="A29" s="2">
         <v>45946.604629629626</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="3">
         <v>26.280000000000001</v>
       </c>
       <c r="C29">
@@ -2344,10 +2344,10 @@
       </c>
     </row>
     <row r="30" ht="14.25">
-      <c r="A30" s="3">
+      <c r="A30" s="2">
         <v>45946.604641203703</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="3">
         <v>26.690000000000001</v>
       </c>
       <c r="C30">
@@ -2355,10 +2355,10 @@
       </c>
     </row>
     <row r="31" ht="14.25">
-      <c r="A31" s="3">
+      <c r="A31" s="2">
         <v>45946.60465277778</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="3">
         <v>26.949999999999999</v>
       </c>
       <c r="C31">
@@ -2366,10 +2366,10 @@
       </c>
     </row>
     <row r="32" ht="14.25">
-      <c r="A32" s="3">
+      <c r="A32" s="2">
         <v>45946.604675925926</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="3">
         <v>27.120000000000001</v>
       </c>
       <c r="C32">
@@ -2377,10 +2377,10 @@
       </c>
     </row>
     <row r="33" ht="14.25">
-      <c r="A33" s="3">
+      <c r="A33" s="2">
         <v>45946.604687500003</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="3">
         <v>27.34</v>
       </c>
       <c r="C33">
@@ -2388,10 +2388,10 @@
       </c>
     </row>
     <row r="34" ht="14.25">
-      <c r="A34" s="3">
+      <c r="A34" s="2">
         <v>45946.604699074072</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B34" s="3">
         <v>27.469999999999999</v>
       </c>
       <c r="C34">
@@ -2399,10 +2399,10 @@
       </c>
     </row>
     <row r="35" ht="14.25">
-      <c r="A35" s="3">
+      <c r="A35" s="2">
         <v>45946.604710648149</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35" s="3">
         <v>27.579999999999998</v>
       </c>
       <c r="C35">
@@ -2410,10 +2410,10 @@
       </c>
     </row>
     <row r="36" ht="14.25">
-      <c r="A36" s="3">
+      <c r="A36" s="2">
         <v>45946.604733796295</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B36" s="3">
         <v>27.710000000000001</v>
       </c>
       <c r="C36">
@@ -2421,10 +2421,10 @@
       </c>
     </row>
     <row r="37" ht="14.25">
-      <c r="A37" s="3">
+      <c r="A37" s="2">
         <v>45946.604745370372</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37" s="3">
         <v>27.82</v>
       </c>
       <c r="C37">
@@ -2432,10 +2432,10 @@
       </c>
     </row>
     <row r="38" ht="14.25">
-      <c r="A38" s="3">
+      <c r="A38" s="2">
         <v>45946.604756944442</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B38" s="3">
         <v>27.93</v>
       </c>
       <c r="C38">
@@ -2443,10 +2443,10 @@
       </c>
     </row>
     <row r="39" ht="14.25">
-      <c r="A39" s="3">
+      <c r="A39" s="2">
         <v>45946.604768518519</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39" s="3">
         <v>27.969999999999999</v>
       </c>
       <c r="C39">
@@ -2454,10 +2454,10 @@
       </c>
     </row>
     <row r="40" ht="14.25">
-      <c r="A40" s="3">
+      <c r="A40" s="2">
         <v>45946.604791666665</v>
       </c>
-      <c r="B40" s="4">
+      <c r="B40" s="3">
         <v>28.059999999999999</v>
       </c>
       <c r="C40">
@@ -2465,10 +2465,10 @@
       </c>
     </row>
     <row r="41" ht="14.25">
-      <c r="A41" s="3">
+      <c r="A41" s="2">
         <v>45946.604803240742</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41" s="3">
         <v>28.149999999999999</v>
       </c>
       <c r="C41">
@@ -2476,10 +2476,10 @@
       </c>
     </row>
     <row r="42" ht="14.25">
-      <c r="A42" s="3">
+      <c r="A42" s="2">
         <v>45946.604814814818</v>
       </c>
-      <c r="B42" s="4">
+      <c r="B42" s="3">
         <v>28.23</v>
       </c>
       <c r="C42">
@@ -2487,10 +2487,10 @@
       </c>
     </row>
     <row r="43" ht="14.25">
-      <c r="A43" s="3">
+      <c r="A43" s="2">
         <v>45946.604826388888</v>
       </c>
-      <c r="B43" s="4">
+      <c r="B43" s="3">
         <v>28.300000000000001</v>
       </c>
       <c r="C43">
@@ -2498,10 +2498,10 @@
       </c>
     </row>
     <row r="44" ht="14.25">
-      <c r="A44" s="3">
+      <c r="A44" s="2">
         <v>45946.604837962965</v>
       </c>
-      <c r="B44" s="4">
+      <c r="B44" s="3">
         <v>28.370000000000001</v>
       </c>
       <c r="C44">
@@ -2509,10 +2509,10 @@
       </c>
     </row>
     <row r="45" ht="14.25">
-      <c r="A45" s="3">
+      <c r="A45" s="2">
         <v>45946.604861111111</v>
       </c>
-      <c r="B45" s="4">
+      <c r="B45" s="3">
         <v>28.420000000000002</v>
       </c>
       <c r="C45">
@@ -2520,10 +2520,10 @@
       </c>
     </row>
     <row r="46" ht="14.25">
-      <c r="A46" s="3">
+      <c r="A46" s="2">
         <v>45946.604872685188</v>
       </c>
-      <c r="B46" s="4">
+      <c r="B46" s="3">
         <v>28.489999999999998</v>
       </c>
       <c r="C46">
@@ -2531,10 +2531,10 @@
       </c>
     </row>
     <row r="47" ht="14.25">
-      <c r="A47" s="3">
+      <c r="A47" s="2">
         <v>45946.604884259257</v>
       </c>
-      <c r="B47" s="4">
+      <c r="B47" s="3">
         <v>28.530000000000001</v>
       </c>
       <c r="C47">
@@ -2542,10 +2542,10 @@
       </c>
     </row>
     <row r="48" ht="14.25">
-      <c r="A48" s="3">
+      <c r="A48" s="2">
         <v>45946.604895833334</v>
       </c>
-      <c r="B48" s="4">
+      <c r="B48" s="3">
         <v>28.579999999999998</v>
       </c>
       <c r="C48">
@@ -2553,10 +2553,10 @@
       </c>
     </row>
     <row r="49" ht="14.25">
-      <c r="A49" s="3">
+      <c r="A49" s="2">
         <v>45946.60491898148</v>
       </c>
-      <c r="B49" s="4">
+      <c r="B49" s="3">
         <v>28.609999999999999</v>
       </c>
       <c r="C49">
@@ -2564,10 +2564,10 @@
       </c>
     </row>
     <row r="50" ht="14.25">
-      <c r="A50" s="3">
+      <c r="A50" s="2">
         <v>45946.604930555557</v>
       </c>
-      <c r="B50" s="4">
+      <c r="B50" s="3">
         <v>28.66</v>
       </c>
       <c r="C50">
@@ -2575,10 +2575,10 @@
       </c>
     </row>
     <row r="51" ht="14.25">
-      <c r="A51" s="3">
+      <c r="A51" s="2">
         <v>45946.604942129627</v>
       </c>
-      <c r="B51" s="4">
+      <c r="B51" s="3">
         <v>28.609999999999999</v>
       </c>
       <c r="C51">
@@ -2586,10 +2586,10 @@
       </c>
     </row>
     <row r="52" ht="14.25">
-      <c r="A52" s="3">
+      <c r="A52" s="2">
         <v>45946.604953703703</v>
       </c>
-      <c r="B52" s="4">
+      <c r="B52" s="3">
         <v>28.350000000000001</v>
       </c>
       <c r="C52">
@@ -2597,10 +2597,10 @@
       </c>
     </row>
     <row r="53" ht="14.25">
-      <c r="A53" s="3">
+      <c r="A53" s="2">
         <v>45946.60496527778</v>
       </c>
-      <c r="B53" s="4">
+      <c r="B53" s="3">
         <v>28.059999999999999</v>
       </c>
       <c r="C53">
@@ -2608,10 +2608,10 @@
       </c>
     </row>
     <row r="54" ht="14.25">
-      <c r="A54" s="3">
+      <c r="A54" s="2">
         <v>45946.604988425926</v>
       </c>
-      <c r="B54" s="4">
+      <c r="B54" s="3">
         <v>27.82</v>
       </c>
       <c r="C54">
@@ -2619,10 +2619,10 @@
       </c>
     </row>
     <row r="55" ht="14.25">
-      <c r="A55" s="3">
+      <c r="A55" s="2">
         <v>45946.605000000003</v>
       </c>
-      <c r="B55" s="4">
+      <c r="B55" s="3">
         <v>27.629999999999999</v>
       </c>
       <c r="C55">
@@ -2630,10 +2630,10 @@
       </c>
     </row>
     <row r="56" ht="14.25">
-      <c r="A56" s="3">
+      <c r="A56" s="2">
         <v>45946.605011574073</v>
       </c>
-      <c r="B56" s="4">
+      <c r="B56" s="3">
         <v>27.489999999999998</v>
       </c>
       <c r="C56">
@@ -2641,10 +2641,10 @@
       </c>
     </row>
     <row r="57" ht="14.25">
-      <c r="A57" s="3">
+      <c r="A57" s="2">
         <v>45946.605023148149</v>
       </c>
-      <c r="B57" s="4">
+      <c r="B57" s="3">
         <v>27.359999999999999</v>
       </c>
       <c r="C57">
@@ -2652,10 +2652,10 @@
       </c>
     </row>
     <row r="58" ht="14.25">
-      <c r="A58" s="3">
+      <c r="A58" s="2">
         <v>45946.605046296296</v>
       </c>
-      <c r="B58" s="4">
+      <c r="B58" s="3">
         <v>27.289999999999999</v>
       </c>
       <c r="C58">
@@ -2663,10 +2663,10 @@
       </c>
     </row>
     <row r="59" ht="14.25">
-      <c r="A59" s="3">
+      <c r="A59" s="2">
         <v>45946.605057870373</v>
       </c>
-      <c r="B59" s="4">
+      <c r="B59" s="3">
         <v>27.190000000000001</v>
       </c>
       <c r="C59">
@@ -2674,10 +2674,10 @@
       </c>
     </row>
     <row r="60" ht="14.25">
-      <c r="A60" s="3">
+      <c r="A60" s="2">
         <v>45946.605069444442</v>
       </c>
-      <c r="B60" s="4">
+      <c r="B60" s="3">
         <v>27.09</v>
       </c>
       <c r="C60">
@@ -2685,10 +2685,10 @@
       </c>
     </row>
     <row r="61" ht="14.25">
-      <c r="A61" s="3">
+      <c r="A61" s="2">
         <v>45946.605081018519</v>
       </c>
-      <c r="B61" s="4">
+      <c r="B61" s="3">
         <v>27.039999999999999</v>
       </c>
       <c r="C61">
@@ -2696,10 +2696,10 @@
       </c>
     </row>
     <row r="62" ht="14.25">
-      <c r="A62" s="3">
+      <c r="A62" s="2">
         <v>45946.605104166665</v>
       </c>
-      <c r="B62" s="4">
+      <c r="B62" s="3">
         <v>26.949999999999999</v>
       </c>
       <c r="C62">
@@ -2707,10 +2707,10 @@
       </c>
     </row>
     <row r="63" ht="14.25">
-      <c r="A63" s="3">
+      <c r="A63" s="2">
         <v>45946.605115740742</v>
       </c>
-      <c r="B63" s="4">
+      <c r="B63" s="3">
         <v>26.91</v>
       </c>
       <c r="C63">
@@ -2718,10 +2718,10 @@
       </c>
     </row>
     <row r="64" ht="14.25">
-      <c r="A64" s="3">
+      <c r="A64" s="2">
         <v>45946.605127314811</v>
       </c>
-      <c r="B64" s="4">
+      <c r="B64" s="3">
         <v>26.829999999999998</v>
       </c>
       <c r="C64">
@@ -2729,10 +2729,10 @@
       </c>
     </row>
     <row r="65" ht="14.25">
-      <c r="A65" s="3">
+      <c r="A65" s="2">
         <v>45946.605138888888</v>
       </c>
-      <c r="B65" s="4">
+      <c r="B65" s="3">
         <v>26.789999999999999</v>
       </c>
       <c r="C65">
@@ -2740,10 +2740,10 @@
       </c>
     </row>
     <row r="66" ht="14.25">
-      <c r="A66" s="3">
+      <c r="A66" s="2">
         <v>45946.605150462965</v>
       </c>
-      <c r="B66" s="4">
+      <c r="B66" s="3">
         <v>26.760000000000002</v>
       </c>
       <c r="C66">
@@ -2751,10 +2751,10 @@
       </c>
     </row>
     <row r="67" ht="14.25">
-      <c r="A67" s="3">
+      <c r="A67" s="2">
         <v>45946.605173611111</v>
       </c>
-      <c r="B67" s="4">
+      <c r="B67" s="3">
         <v>26.68</v>
       </c>
       <c r="C67">
@@ -2762,10 +2762,10 @@
       </c>
     </row>
     <row r="68" ht="14.25">
-      <c r="A68" s="3">
+      <c r="A68" s="2">
         <v>45946.605185185188</v>
       </c>
-      <c r="B68" s="4">
+      <c r="B68" s="3">
         <v>26.640000000000001</v>
       </c>
       <c r="C68">
@@ -2773,10 +2773,10 @@
       </c>
     </row>
     <row r="69" ht="14.25">
-      <c r="A69" s="3">
+      <c r="A69" s="2">
         <v>45946.605196759258</v>
       </c>
-      <c r="B69" s="4">
+      <c r="B69" s="3">
         <v>26.609999999999999</v>
       </c>
       <c r="C69">
@@ -2784,10 +2784,10 @@
       </c>
     </row>
     <row r="70" ht="14.25">
-      <c r="A70" s="3">
+      <c r="A70" s="2">
         <v>45946.605208333334</v>
       </c>
-      <c r="B70" s="4">
+      <c r="B70" s="3">
         <v>26.559999999999999</v>
       </c>
       <c r="C70">
@@ -2795,10 +2795,10 @@
       </c>
     </row>
     <row r="71" ht="14.25">
-      <c r="A71" s="3">
+      <c r="A71" s="2">
         <v>45946.605231481481</v>
       </c>
-      <c r="B71" s="4">
+      <c r="B71" s="3">
         <v>26.559999999999999</v>
       </c>
       <c r="C71">
@@ -2806,10 +2806,10 @@
       </c>
     </row>
     <row r="72" ht="14.25">
-      <c r="A72" s="3">
+      <c r="A72" s="2">
         <v>45946.605243055557</v>
       </c>
-      <c r="B72" s="4">
+      <c r="B72" s="3">
         <v>26.5</v>
       </c>
       <c r="C72">
@@ -2817,10 +2817,10 @@
       </c>
     </row>
     <row r="73" ht="14.25">
-      <c r="A73" s="3">
+      <c r="A73" s="2">
         <v>45946.605254629627</v>
       </c>
-      <c r="B73" s="4">
+      <c r="B73" s="3">
         <v>26.48</v>
       </c>
       <c r="C73">
@@ -2828,10 +2828,10 @@
       </c>
     </row>
     <row r="74" ht="14.25">
-      <c r="A74" s="3">
+      <c r="A74" s="2">
         <v>45946.605266203704</v>
       </c>
-      <c r="B74" s="4">
+      <c r="B74" s="3">
         <v>26.440000000000001</v>
       </c>
       <c r="C74">

</xml_diff>